<commit_message>
HomepageUser sign in Test Data (Including valid and invalid scenarios) Test xml file
</commit_message>
<xml_diff>
--- a/TestData/SigninTestData.xlsx
+++ b/TestData/SigninTestData.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\QA\My QA Projects\mageplaza-Ecommerce-Site-Test\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\QA\My QA Projects\Mageplaza-Ecommerce-Site-Test\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BACE868F-DC2A-4CE3-AC3A-C29EF59BF13C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{241D06F5-CC68-4815-AE82-9E5D7E2EBDDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{EF069275-26B5-4974-84B8-DE96466304A7}"/>
   </bookViews>
@@ -430,12 +430,12 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.33203125" customWidth="1"/>
+    <col min="1" max="1" width="25.33203125" customWidth="1"/>
     <col min="2" max="2" width="12.33203125" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>

<commit_message>
User sign in Test Data (Including valid and invalid scenarios) Test xml file
</commit_message>
<xml_diff>
--- a/TestData/SigninTestData.xlsx
+++ b/TestData/SigninTestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\QA\My QA Projects\Mageplaza-Ecommerce-Site-Test\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{241D06F5-CC68-4815-AE82-9E5D7E2EBDDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F7781D7-0788-4CA3-ADD5-134FB06E6D25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{EF069275-26B5-4974-84B8-DE96466304A7}"/>
   </bookViews>
@@ -430,12 +430,12 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="25.33203125" customWidth="1"/>
+    <col min="1" max="1" width="22.6640625" customWidth="1"/>
     <col min="2" max="2" width="12.33203125" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>